<commit_message>
Set of costs added to the objective
FlowThinning_Esati.py - is the python code for FT formulation problem. Cost function it is added the the objective.
AffineFlowThinning_Esati.py - is the python code for AFT formulation problem. Cost function it is added the the objective.
example.xlsx - is the excel file that contains the input data for the example problem (from task 1.2). Cos function is added in an extra sheet.

Results_FlowThinning.xlsx - The decision variables are printed in this excel file for FT problem.
Results_AffineFlowThinning.xlsx  - The decision variables are printed in this excel file for AFT problem.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8325" windowHeight="6705" tabRatio="705" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8325" windowHeight="6705" tabRatio="705" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="IPnodes" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Paths R(d,e)" sheetId="16" r:id="rId10"/>
     <sheet name="subset states" sheetId="17" r:id="rId11"/>
     <sheet name="Alpha" sheetId="18" r:id="rId12"/>
-    <sheet name="test" sheetId="20" r:id="rId13"/>
-    <sheet name="Links E(d,p)" sheetId="11" r:id="rId14"/>
+    <sheet name="Links E(d,p)" sheetId="11" r:id="rId13"/>
+    <sheet name="Cost" sheetId="21" r:id="rId14"/>
     <sheet name="Beta" sheetId="19" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="94">
   <si>
     <t>IP links E</t>
   </si>
@@ -314,184 +314,7 @@
     <t>0.8</t>
   </si>
   <si>
-    <t>p115,p116,p117</t>
-  </si>
-  <si>
-    <t>p118,p119</t>
-  </si>
-  <si>
-    <t>p120</t>
-  </si>
-  <si>
-    <t>p121</t>
-  </si>
-  <si>
-    <t>p122</t>
-  </si>
-  <si>
-    <t>p123</t>
-  </si>
-  <si>
-    <t>p124</t>
-  </si>
-  <si>
-    <t>p125,p126,p127</t>
-  </si>
-  <si>
-    <t>p128</t>
-  </si>
-  <si>
-    <t>p129</t>
-  </si>
-  <si>
-    <t>p130</t>
-  </si>
-  <si>
-    <t>p131,p132,p133</t>
-  </si>
-  <si>
-    <t>p134</t>
-  </si>
-  <si>
-    <t>p135</t>
-  </si>
-  <si>
-    <t>p136</t>
-  </si>
-  <si>
-    <t>p137</t>
-  </si>
-  <si>
-    <t>p138,p139</t>
-  </si>
-  <si>
-    <t>p140</t>
-  </si>
-  <si>
-    <t>p141,p142</t>
-  </si>
-  <si>
-    <t>p143</t>
-  </si>
-  <si>
-    <t>p144,p145,p146</t>
-  </si>
-  <si>
-    <t>p147,p148,p149</t>
-  </si>
-  <si>
-    <t>p150,p151</t>
-  </si>
-  <si>
-    <t>p152</t>
-  </si>
-  <si>
-    <t>p153,p154,p155</t>
-  </si>
-  <si>
-    <t>p156</t>
-  </si>
-  <si>
-    <t>p157,p158</t>
-  </si>
-  <si>
-    <t>p159,p160</t>
-  </si>
-  <si>
-    <t>p161,p162</t>
-  </si>
-  <si>
-    <t>p163</t>
-  </si>
-  <si>
-    <t>p164</t>
-  </si>
-  <si>
-    <t>p165,p166</t>
-  </si>
-  <si>
-    <t>p167,p168</t>
-  </si>
-  <si>
-    <t>p169</t>
-  </si>
-  <si>
-    <t>p170</t>
-  </si>
-  <si>
-    <t>p171,p172,p173</t>
-  </si>
-  <si>
-    <t>p174</t>
-  </si>
-  <si>
-    <t>p175,p176</t>
-  </si>
-  <si>
-    <t>p177,p178</t>
-  </si>
-  <si>
-    <t>p179,p180,p181</t>
-  </si>
-  <si>
-    <t>p182</t>
-  </si>
-  <si>
-    <t>p183</t>
-  </si>
-  <si>
-    <t>p184,p185</t>
-  </si>
-  <si>
-    <t>p186,p187</t>
-  </si>
-  <si>
-    <t>p188</t>
-  </si>
-  <si>
-    <t>p189</t>
-  </si>
-  <si>
-    <t>p190</t>
-  </si>
-  <si>
-    <t>p191</t>
-  </si>
-  <si>
-    <t>p192,p193</t>
-  </si>
-  <si>
-    <t>p194,p195</t>
-  </si>
-  <si>
-    <t>p196,p197</t>
-  </si>
-  <si>
-    <t>p198</t>
-  </si>
-  <si>
-    <t>p199</t>
-  </si>
-  <si>
-    <t>p200,p201</t>
-  </si>
-  <si>
-    <t>p204</t>
-  </si>
-  <si>
-    <t>p202,p203</t>
-  </si>
-  <si>
-    <t>p205</t>
-  </si>
-  <si>
-    <t>p206,p207</t>
-  </si>
-  <si>
-    <t>p208,p209</t>
-  </si>
-  <si>
-    <t>p210,p211</t>
+    <t>unit cost of IP link</t>
   </si>
 </sst>
 </file>
@@ -932,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,535 +1188,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B69"/>
-  <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="24.140625" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
-        <v>73</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>76</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>77</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>78</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>79</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>80</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>81</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>82</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>83</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>85</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>86</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>87</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>88</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>89</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>90</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>91</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>92</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>93</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>94</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>95</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>96</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>97</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>98</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>99</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>100</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>101</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>102</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>103</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>104</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>105</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>106</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>107</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>108</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>109</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>110</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>111</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>112</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>113</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>114</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>115</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>116</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>117</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>118</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>119</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>120</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>121</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>122</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>123</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>124</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>125</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>126</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>127</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
-        <v>128</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
-        <v>129</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
-        <v>130</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
-        <v>131</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>132</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,6 +1388,56 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2606,7 +1954,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,7 +2384,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>